<commit_message>
Revert "[PdP] - Dati Preventivo (sez.4), Prospetto Economico (sez.5) e Suddivisione del lavoro (sez.6) aggiornati. Aggiornate relative immagini. TODO: 1) Aggiornare Analisi dei Rischi, 2) Aggiornare Consuntivo, 3) Aggiornare Organigramma, 4) Sistemare Diario, 5) Sistemare intestazione documento."
This reverts commit 26f44c666703c1ffd2e84966613a0095e5748ba9.
</commit_message>
<xml_diff>
--- a/4 - RA/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
+++ b/4 - RA/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbazzerl/Desktop/SWE/MonolithGitHub/documenti/4 - RA/Esterni/Piano Di Progetto/GANTT-EXCEL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fbazzerl/Desktop/SWE/MonolithGitHub/documenti/3 - RQ/Esterni/Piano Di Progetto/GANTT-EXCEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13800" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ARM" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="32">
   <si>
     <t>Francesco Bazzerla</t>
   </si>
@@ -131,15 +131,12 @@
   <si>
     <t>Programmatore</t>
   </si>
-  <si>
-    <t>2-1+0+21+7+6</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,6 +196,11 @@
       <name val="TeXGyreHeros"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="TeXGyreHeros"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -208,22 +210,6 @@
     <font>
       <sz val="11"/>
       <name val="TeXGyreHeros"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -272,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -294,28 +280,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -870,11 +853,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2110531856"/>
-        <c:axId val="2110535408"/>
+        <c:axId val="-2133680032"/>
+        <c:axId val="-2133677440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110531856"/>
+        <c:axId val="-2133680032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +900,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110535408"/>
+        <c:crossAx val="-2133677440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -925,7 +908,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110535408"/>
+        <c:axId val="-2133677440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -976,7 +959,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110531856"/>
+        <c:crossAx val="-2133680032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2019,11 +2002,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109892272"/>
-        <c:axId val="2109843472"/>
+        <c:axId val="-2132633616"/>
+        <c:axId val="-2133578032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109892272"/>
+        <c:axId val="-2132633616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2066,7 +2049,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109843472"/>
+        <c:crossAx val="-2133578032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2074,7 +2057,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109843472"/>
+        <c:axId val="-2133578032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2125,7 +2108,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109892272"/>
+        <c:crossAx val="-2132633616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2139,7 +2122,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3165,7 +3147,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>9.0</c:v>
@@ -3249,7 +3231,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4.0</c:v>
@@ -3402,16 +3384,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>16.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.0</c:v>
@@ -3492,19 +3474,19 @@
                   <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3570,25 +3552,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3604,11 +3586,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2112092592"/>
-        <c:axId val="2112096128"/>
+        <c:axId val="-2134429040"/>
+        <c:axId val="-2134479904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2112092592"/>
+        <c:axId val="-2134429040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3651,7 +3633,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112096128"/>
+        <c:crossAx val="-2134479904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3659,7 +3641,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112096128"/>
+        <c:axId val="-2134479904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3710,7 +3692,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112092592"/>
+        <c:crossAx val="-2134429040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3724,7 +3706,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4567,9 +4548,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4588,9 +4567,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4660,9 +4637,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4755,7 +4730,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -4921,7 +4895,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>9.0</c:v>
@@ -5005,7 +4979,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>6.0</c:v>
@@ -5158,16 +5132,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>21.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7.0</c:v>
@@ -5248,19 +5222,19 @@
                   <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5326,25 +5300,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>14.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5360,11 +5334,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109755664"/>
-        <c:axId val="2109752320"/>
+        <c:axId val="-2133388912"/>
+        <c:axId val="-2133385360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109755664"/>
+        <c:axId val="-2133388912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5407,7 +5381,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109752320"/>
+        <c:crossAx val="-2133385360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5415,7 +5389,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109752320"/>
+        <c:axId val="-2133385360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5466,7 +5440,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109755664"/>
+        <c:crossAx val="-2133388912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5480,7 +5454,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5780,9 +5753,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5852,9 +5823,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -5947,7 +5916,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6250,9 +6218,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6322,9 +6288,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6366,10 +6330,10 @@
                   <c:v>2354.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2160.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1875.0</c:v>
+                  <c:v>2085.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6417,7 +6381,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6754,9 +6717,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6839,7 +6800,6 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6990,22 +6950,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -7080,7 +7040,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -7092,7 +7052,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7251,10 +7211,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.0</c:v>
@@ -7326,7 +7286,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -7335,16 +7295,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7410,25 +7370,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7444,11 +7404,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2112208960"/>
-        <c:axId val="2112212512"/>
+        <c:axId val="-2133232432"/>
+        <c:axId val="-2133228896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2112208960"/>
+        <c:axId val="-2133232432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7491,7 +7451,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112212512"/>
+        <c:crossAx val="-2133228896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7499,7 +7459,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112212512"/>
+        <c:axId val="-2133228896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7550,7 +7510,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112208960"/>
+        <c:crossAx val="-2133232432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8353,7 +8313,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -8377,7 +8336,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8414,7 +8372,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8422,7 +8379,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -8446,7 +8402,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8454,7 +8409,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -8478,7 +8432,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -8699,7 +8652,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -10036,22 +9988,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>10.0</c:v>
@@ -10126,7 +10078,7 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>5.0</c:v>
@@ -10135,10 +10087,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10288,19 +10240,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="1">
-                  <c:v>41.0</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42.0</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>26.0</c:v>
@@ -10378,16 +10330,16 @@
                   <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.0</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>22.0</c:v>
@@ -10456,25 +10408,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="1">
-                  <c:v>28.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44.0</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.0</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.0</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>48.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42.0</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>29.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10490,11 +10442,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2112456672"/>
-        <c:axId val="2112460240"/>
+        <c:axId val="-2133115328"/>
+        <c:axId val="-2133111760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2112456672"/>
+        <c:axId val="-2133115328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10537,7 +10489,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112460240"/>
+        <c:crossAx val="-2133111760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10545,7 +10497,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112460240"/>
+        <c:axId val="-2133111760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10596,7 +10548,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112456672"/>
+        <c:crossAx val="-2133115328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10610,7 +10562,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11066,7 +11017,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -11476,11 +11429,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2113465408"/>
-        <c:axId val="2113468336"/>
+        <c:axId val="-2036624208"/>
+        <c:axId val="-2061523200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2113465408"/>
+        <c:axId val="-2036624208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11490,7 +11443,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113468336"/>
+        <c:crossAx val="-2061523200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11498,7 +11451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113468336"/>
+        <c:axId val="-2061523200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11561,7 +11514,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2113465408"/>
+        <c:crossAx val="-2036624208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11907,9 +11860,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -12000,7 +11951,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -12114,6 +12064,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12664,11 +12615,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109678768"/>
-        <c:axId val="2109682304"/>
+        <c:axId val="-2136936240"/>
+        <c:axId val="-2136939792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109678768"/>
+        <c:axId val="-2136936240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12711,7 +12662,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109682304"/>
+        <c:crossAx val="-2136939792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12719,7 +12670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109682304"/>
+        <c:axId val="-2136939792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12770,7 +12721,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109678768"/>
+        <c:crossAx val="-2136936240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12784,6 +12735,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13025,6 +12977,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -13100,11 +13053,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="2108927104"/>
-        <c:axId val="2108923456"/>
+        <c:axId val="-2135438128"/>
+        <c:axId val="-2135434496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2108927104"/>
+        <c:axId val="-2135438128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13142,7 +13095,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108923456"/>
+        <c:crossAx val="-2135434496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13150,7 +13103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108923456"/>
+        <c:axId val="-2135434496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13213,7 +13166,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108927104"/>
+        <c:crossAx val="-2135438128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13791,11 +13744,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2110745760"/>
-        <c:axId val="2110749296"/>
+        <c:axId val="-2133560560"/>
+        <c:axId val="-2133557008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110745760"/>
+        <c:axId val="-2133560560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13838,7 +13791,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110749296"/>
+        <c:crossAx val="-2133557008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13846,7 +13799,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110749296"/>
+        <c:axId val="-2133557008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13897,7 +13850,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110745760"/>
+        <c:crossAx val="-2133560560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13911,7 +13864,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14932,11 +14884,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109954704"/>
-        <c:axId val="2109951152"/>
+        <c:axId val="-2133543168"/>
+        <c:axId val="-2133539632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109954704"/>
+        <c:axId val="-2133543168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14979,7 +14931,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109951152"/>
+        <c:crossAx val="-2133539632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14987,7 +14939,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109951152"/>
+        <c:axId val="-2133539632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15038,7 +14990,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109954704"/>
+        <c:crossAx val="-2133543168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15052,7 +15004,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -34287,8 +34238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A79" zoomScale="83" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView showRuler="0" zoomScale="83" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34542,52 +34493,52 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="9">
         <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="9">
         <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="9">
         <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="9">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
@@ -34595,81 +34546,81 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B83" s="10">
+      <c r="B83" s="9">
         <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="11"/>
-      <c r="B84" s="10"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="9"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B85" s="10">
+      <c r="B85" s="9">
         <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="11"/>
-      <c r="B86" s="10"/>
+      <c r="A86" s="10"/>
+      <c r="B86" s="9"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="11" t="s">
+      <c r="A87" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B87" s="10">
+      <c r="B87" s="9">
         <v>750</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="11"/>
-      <c r="B88" s="10"/>
+      <c r="A88" s="10"/>
+      <c r="B88" s="9"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="11" t="s">
+      <c r="A89" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B89" s="10">
+      <c r="B89" s="9">
         <v>210</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="11"/>
-      <c r="B90" s="10"/>
+      <c r="A90" s="10"/>
+      <c r="B90" s="9"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="9"/>
-      <c r="B91" s="10"/>
+      <c r="A91" s="11"/>
+      <c r="B91" s="9"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="9"/>
-      <c r="B92" s="10"/>
+      <c r="A92" s="11"/>
+      <c r="B92" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="B89:B90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -34678,21 +34629,17 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7">
-        <f>26+7</f>
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B1" s="7">
         <v>28</v>
@@ -34701,30 +34648,19 @@
         <v>17</v>
       </c>
       <c r="D1" s="8">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F1">
         <f t="shared" ref="F1:F7" si="0">SUM(A1:E1)</f>
-        <v>141</v>
-      </c>
-      <c r="G1">
-        <f>F1-36</f>
-        <v>105</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
-        <f>26+7</f>
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B2" s="7">
         <v>28</v>
@@ -34733,30 +34669,19 @@
         <v>17</v>
       </c>
       <c r="D2" s="8">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <f t="shared" si="0"/>
-        <v>141</v>
-      </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G7" si="1">F2-36</f>
-        <v>105</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
-        <f>25+8</f>
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B3" s="7">
         <v>28</v>
@@ -34765,30 +34690,19 @@
         <v>18</v>
       </c>
       <c r="D3" s="8">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="G3">
-        <f>F3-35</f>
-        <v>105</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
-        <f>26+7</f>
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B4" s="7">
         <v>28</v>
@@ -34797,30 +34711,19 @@
         <v>17</v>
       </c>
       <c r="D4" s="8">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E4">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>141</v>
-      </c>
-      <c r="G4">
-        <f>F4-36</f>
-        <v>105</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
-        <f>25+7</f>
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B5" s="7">
         <v>29</v>
@@ -34829,30 +34732,19 @@
         <v>17</v>
       </c>
       <c r="D5" s="8">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E5">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="G5">
-        <f>F5-35</f>
-        <v>105</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
-        <f>26+7</f>
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B6" s="7">
         <v>28</v>
@@ -34861,30 +34753,19 @@
         <v>18</v>
       </c>
       <c r="D6" s="8">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E6">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="G6" s="23">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="23">
-        <v>-1</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
-        <f>25+7</f>
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B7" s="7">
         <v>29</v>
@@ -34893,24 +34774,14 @@
         <v>17</v>
       </c>
       <c r="D7" s="8">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="G7">
-        <f>F7-35</f>
-        <v>105</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -34922,145 +34793,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:D43"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="C3" zoomScaleNormal="187" zoomScalePageLayoutView="187" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F32" zoomScaleNormal="187" zoomScalePageLayoutView="187" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="4" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>53</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C35" s="10"/>
-      <c r="D35" s="15"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="13"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="13">
         <v>-1</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C37" s="10"/>
-      <c r="D37" s="15"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="13"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="13">
         <v>21</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C39" s="10"/>
-      <c r="D39" s="15"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="13"/>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="23">
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C41" s="10"/>
-      <c r="D41" s="22"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="23"/>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D42" s="23">
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C43" s="10"/>
-      <c r="D43" s="22"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C34:C35"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C42:C43"/>
@@ -35069,7 +34929,18 @@
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="D42:D43"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C34:C35"/>
     <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -35139,7 +35010,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="178" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35393,52 +35264,52 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="9">
         <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="10">
+      <c r="B55" s="9">
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -35461,7 +35332,7 @@
   <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35715,103 +35586,111 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="9">
         <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="9">
         <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B80" s="10">
+      <c r="B80" s="9">
         <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="11"/>
-      <c r="B81" s="10"/>
+      <c r="A81" s="10"/>
+      <c r="B81" s="9"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="10">
+      <c r="B82" s="9">
         <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="11"/>
-      <c r="B83" s="10"/>
+      <c r="A83" s="10"/>
+      <c r="B83" s="9"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="11" t="s">
+      <c r="A84" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B84" s="10">
+      <c r="B84" s="9">
         <v>2640</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="11"/>
-      <c r="B85" s="10"/>
+      <c r="A85" s="10"/>
+      <c r="B85" s="9"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="11" t="s">
+      <c r="A86" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B86" s="10">
+      <c r="B86" s="9">
         <v>975</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="11"/>
-      <c r="B87" s="10"/>
+      <c r="A87" s="10"/>
+      <c r="B87" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B82:B83"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A43:A44"/>
@@ -35820,14 +35699,6 @@
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B82:B83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -35839,7 +35710,7 @@
   <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="124" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36093,103 +35964,111 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="9">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="10">
+      <c r="B55" s="9">
         <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="11" t="s">
+      <c r="A86" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B86" s="10">
+      <c r="B86" s="9">
         <v>210</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="11"/>
-      <c r="B87" s="10"/>
+      <c r="A87" s="10"/>
+      <c r="B87" s="9"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B88" s="10">
+      <c r="B88" s="9">
         <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="11"/>
-      <c r="B89" s="10"/>
+      <c r="A89" s="10"/>
+      <c r="B89" s="9"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B90" s="10">
+      <c r="B90" s="9">
         <v>1430</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="11"/>
-      <c r="B91" s="10"/>
+      <c r="A91" s="10"/>
+      <c r="B91" s="9"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="11" t="s">
+      <c r="A92" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B92" s="10">
+      <c r="B92" s="9">
         <v>630</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="11"/>
-      <c r="B93" s="10"/>
+      <c r="A93" s="10"/>
+      <c r="B93" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="A49:A50"/>
@@ -36198,14 +36077,6 @@
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="A53:A54"/>
     <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -36214,19 +36085,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A66" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView showRuler="0" topLeftCell="A40" zoomScale="135" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -36252,7 +36122,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -36266,20 +36136,20 @@
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F2" s="4">
         <v>30</v>
       </c>
       <c r="G2" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H2" s="4">
         <f>SUM(B2:G2)</f>
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -36293,7 +36163,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F3" s="4">
         <v>24</v>
@@ -36303,10 +36173,10 @@
       </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H8" si="0">SUM(B3:G3)</f>
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -36320,20 +36190,20 @@
         <v>0</v>
       </c>
       <c r="E4" s="4">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F4" s="4">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -36347,7 +36217,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F5" s="4">
         <v>22</v>
@@ -36357,10 +36227,10 @@
       </c>
       <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -36377,28 +36247,25 @@
         <v>0</v>
       </c>
       <c r="F6" s="4">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G6" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="J6" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
         <v>2</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
@@ -36410,14 +36277,14 @@
         <v>31</v>
       </c>
       <c r="G7" s="4">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -36434,24 +36301,24 @@
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="4">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" ref="B9:H9" si="1">SUM(B2:B8)</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
@@ -36459,19 +36326,19 @@
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="1"/>
-        <v>357</v>
+        <v>322</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -36488,161 +36355,175 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="9">
         <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="9">
         <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="9">
         <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="9">
         <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B77" s="10">
+      <c r="B77" s="9">
         <v>390</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="11"/>
-      <c r="B78" s="10"/>
+      <c r="A78" s="10"/>
+      <c r="B78" s="9"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="10">
+      <c r="B79" s="9">
         <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="11"/>
-      <c r="B80" s="10"/>
+      <c r="A80" s="10"/>
+      <c r="B80" s="9"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B81" s="10">
+      <c r="B81" s="9">
         <f>462*2</f>
         <v>924</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="11"/>
-      <c r="B82" s="10"/>
+      <c r="A82" s="10"/>
+      <c r="B82" s="9"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B83" s="10">
+      <c r="B83" s="9">
         <v>2160</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="11"/>
-      <c r="B84" s="10"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="9"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B85" s="10">
+      <c r="B85" s="9">
         <f>1155+90</f>
         <v>1245</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="11"/>
-      <c r="B86" s="10"/>
+      <c r="A86" s="10"/>
+      <c r="B86" s="9"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B97" s="10">
+      <c r="B97" s="9">
         <v>210</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B98" s="10"/>
+      <c r="B98" s="9"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B99" s="10">
+      <c r="B99" s="9">
         <v>140</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B100" s="10"/>
+      <c r="B100" s="9"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B101" s="10">
+      <c r="B101" s="9">
         <v>1430</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B102" s="10"/>
+      <c r="B102" s="9"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B103" s="10">
+      <c r="B103" s="9">
         <v>630</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B104" s="10"/>
+      <c r="B104" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="A51:A52"/>
@@ -36653,20 +36534,6 @@
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B85:B86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -36677,8 +36544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A50" zoomScale="138" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView showRuler="0" zoomScale="138" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36726,17 +36593,17 @@
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F2" s="4">
         <v>30</v>
       </c>
       <c r="G2" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="4">
         <f>SUM(B2:G2)</f>
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -36753,7 +36620,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="4">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F3" s="4">
         <v>24</v>
@@ -36763,7 +36630,7 @@
       </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H8" si="0">SUM(B3:G3)</f>
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -36780,17 +36647,17 @@
         <v>0</v>
       </c>
       <c r="E4" s="4">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F4" s="4">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -36807,7 +36674,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="4">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F5" s="4">
         <v>22</v>
@@ -36817,7 +36684,7 @@
       </c>
       <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -36837,14 +36704,14 @@
         <v>7</v>
       </c>
       <c r="F6" s="4">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G6" s="4">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -36852,10 +36719,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
         <v>2</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
@@ -36867,11 +36734,11 @@
         <v>31</v>
       </c>
       <c r="G7" s="4">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -36891,24 +36758,24 @@
         <v>15</v>
       </c>
       <c r="F8" s="4">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="4">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" ref="B9:H9" si="1">SUM(B2:B8)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
@@ -36916,19 +36783,19 @@
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="1"/>
-        <v>478</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -36940,139 +36807,127 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="9">
         <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="9">
         <v>600</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="11"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B38" s="9">
         <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="9"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="9">
         <v>2354</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="11"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="10">
-        <v>2160</v>
+      <c r="B42" s="9">
+        <v>3000</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="11"/>
-      <c r="B43" s="10"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="9"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="10">
-        <v>1875</v>
+      <c r="B44" s="9">
+        <v>2085</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="11"/>
-      <c r="B45" s="10"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="A38:A39"/>
@@ -37081,6 +36936,18 @@
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -37091,8 +36958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="113" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView showRuler="0" topLeftCell="D37" zoomScale="113" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37131,7 +36998,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4">
         <v>0</v>
@@ -37143,14 +37010,14 @@
         <v>0</v>
       </c>
       <c r="F2" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H2" s="4">
         <f>SUM(B2:G2)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -37158,7 +37025,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4">
         <v>0</v>
@@ -37173,11 +37040,11 @@
         <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H3" s="4">
         <f t="shared" ref="H3:H8" si="0">SUM(B3:G3)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -37188,7 +37055,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -37200,11 +37067,11 @@
         <v>0</v>
       </c>
       <c r="G4" s="4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -37212,7 +37079,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
@@ -37221,17 +37088,17 @@
         <v>0</v>
       </c>
       <c r="E5" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F5" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G5" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -37248,17 +37115,17 @@
         <v>0</v>
       </c>
       <c r="E6" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
       </c>
       <c r="G6" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -37266,7 +37133,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="4">
         <v>0</v>
@@ -37278,14 +37145,14 @@
         <v>3</v>
       </c>
       <c r="F7" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -37296,7 +37163,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -37305,24 +37172,24 @@
         <v>3</v>
       </c>
       <c r="F8" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="4">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" ref="B9:H9" si="1">SUM(B2:B8)</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <f>SUM(C2:C8)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
@@ -37330,19 +37197,19 @@
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -37403,131 +37270,141 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B38" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
-      <c r="B45" s="10"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="9"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B46" s="14">
         <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="10"/>
-      <c r="B47" s="13"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="14"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B75" s="10">
+      <c r="B75" s="9">
         <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="10"/>
+      <c r="B76" s="9"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B77" s="10">
+      <c r="B77" s="9">
         <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="11"/>
-      <c r="B78" s="10"/>
+      <c r="A78" s="10"/>
+      <c r="B78" s="9"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="10">
+      <c r="B79" s="9">
         <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="11"/>
-      <c r="B80" s="10"/>
+      <c r="A80" s="10"/>
+      <c r="B80" s="9"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B81" s="10">
+      <c r="B81" s="9">
         <v>795</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="11"/>
-      <c r="B82" s="10"/>
+      <c r="A82" s="10"/>
+      <c r="B82" s="9"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B83" s="13">
+      <c r="B83" s="14">
         <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="11"/>
-      <c r="B84" s="13"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="14"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="12"/>
+      <c r="A86" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="B81:B82"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="A38:A39"/>
@@ -37538,16 +37415,6 @@
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="B81:B82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -37557,157 +37424,157 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K109"/>
+  <dimension ref="A3:L109"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D88" workbookViewId="0">
-      <selection activeCell="K106" sqref="K106:K107"/>
+    <sheetView showRuler="0" topLeftCell="G5" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="9">
         <v>1110</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="11"/>
-      <c r="B44" s="10"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="9"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="9">
         <v>500</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="11"/>
-      <c r="B46" s="10"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="9"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="9">
         <v>750</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="11"/>
-      <c r="B48" s="10"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="9"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="9">
         <v>5126</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="11"/>
-      <c r="B50" s="10"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="9"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="9">
         <v>2280</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="11"/>
-      <c r="B52" s="10"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="9"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="9">
         <v>3855</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="11"/>
-      <c r="B54" s="10"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="9"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
@@ -37894,43 +37761,43 @@
       </c>
     </row>
     <row r="94" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E94" s="18" t="s">
+      <c r="E94" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F94" s="18" t="s">
+      <c r="F94" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G94" s="18" t="s">
+      <c r="G94" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H94" s="18" t="s">
+      <c r="H94" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="I94" s="18" t="s">
+      <c r="I94" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="J94" s="18" t="s">
+      <c r="J94" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K94" s="20" t="s">
+      <c r="K94" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="95" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E95" s="18"/>
-      <c r="F95" s="18"/>
-      <c r="G95" s="18"/>
-      <c r="H95" s="18"/>
-      <c r="I95" s="18"/>
-      <c r="J95" s="18"/>
-      <c r="K95" s="20"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="20"/>
+      <c r="H95" s="20"/>
+      <c r="I95" s="20"/>
+      <c r="J95" s="20"/>
+      <c r="K95" s="22"/>
     </row>
     <row r="96" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E96" s="19" t="s">
+      <c r="E96" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F96" s="16">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G96" s="16">
         <v>0</v>
@@ -37939,30 +37806,34 @@
         <v>6</v>
       </c>
       <c r="I96" s="16">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J96" s="16">
         <v>22</v>
       </c>
-      <c r="K96" s="17">
-        <v>28</v>
+      <c r="K96" s="19">
+        <v>31</v>
       </c>
     </row>
-    <row r="97" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E97" s="19"/>
+    <row r="97" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E97" s="21"/>
       <c r="F97" s="16"/>
       <c r="G97" s="16"/>
       <c r="H97" s="16"/>
       <c r="I97" s="16"/>
       <c r="J97" s="16"/>
-      <c r="K97" s="17"/>
+      <c r="K97" s="19"/>
+      <c r="L97">
+        <f>SUM(F96:K97)</f>
+        <v>104</v>
+      </c>
     </row>
-    <row r="98" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E98" s="21" t="s">
+    <row r="98" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E98" s="18" t="s">
         <v>24</v>
       </c>
       <c r="F98" s="16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G98" s="16">
         <v>3</v>
@@ -37971,62 +37842,70 @@
         <v>6</v>
       </c>
       <c r="I98" s="16">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="J98" s="16">
         <v>16</v>
       </c>
       <c r="K98" s="17">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="99" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E99" s="21"/>
+    <row r="99" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E99" s="18"/>
       <c r="F99" s="16"/>
       <c r="G99" s="16"/>
       <c r="H99" s="16"/>
       <c r="I99" s="16"/>
       <c r="J99" s="16"/>
       <c r="K99" s="17"/>
+      <c r="L99">
+        <f>SUM(F98:K99)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="100" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E100" s="21" t="s">
+    <row r="100" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E100" s="18" t="s">
         <v>25</v>
       </c>
       <c r="F100" s="16">
         <v>4</v>
       </c>
       <c r="G100" s="16">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H100" s="16">
         <v>0</v>
       </c>
       <c r="I100" s="16">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J100" s="16">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K100" s="17">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="101" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E101" s="21"/>
+    <row r="101" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E101" s="18"/>
       <c r="F101" s="16"/>
       <c r="G101" s="16"/>
       <c r="H101" s="16"/>
       <c r="I101" s="16"/>
       <c r="J101" s="16"/>
       <c r="K101" s="17"/>
+      <c r="L101">
+        <f>SUM(F100:K101)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="102" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E102" s="21" t="s">
+    <row r="102" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E102" s="18" t="s">
         <v>26</v>
       </c>
       <c r="F102" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G102" s="16">
         <v>5</v>
@@ -38035,26 +37914,30 @@
         <v>7</v>
       </c>
       <c r="I102" s="16">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J102" s="16">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K102" s="17">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="103" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E103" s="21"/>
+    <row r="103" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E103" s="18"/>
       <c r="F103" s="16"/>
       <c r="G103" s="16"/>
       <c r="H103" s="16"/>
       <c r="I103" s="16"/>
       <c r="J103" s="16"/>
       <c r="K103" s="17"/>
+      <c r="L103">
+        <f>SUM(F102:K103)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="104" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E104" s="21" t="s">
+    <row r="104" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E104" s="18" t="s">
         <v>27</v>
       </c>
       <c r="F104" s="16">
@@ -38067,33 +37950,37 @@
         <v>6</v>
       </c>
       <c r="I104" s="16">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J104" s="16">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K104" s="17">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="105" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E105" s="21"/>
+    <row r="105" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E105" s="18"/>
       <c r="F105" s="16"/>
       <c r="G105" s="16"/>
       <c r="H105" s="16"/>
       <c r="I105" s="16"/>
       <c r="J105" s="16"/>
       <c r="K105" s="17"/>
+      <c r="L105">
+        <f>SUM(F104:K105)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="106" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E106" s="21" t="s">
+    <row r="106" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E106" s="18" t="s">
         <v>28</v>
       </c>
       <c r="F106" s="16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G106" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H106" s="16">
         <v>5</v>
@@ -38102,30 +37989,34 @@
         <v>26</v>
       </c>
       <c r="J106" s="16">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K106" s="17">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="107" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E107" s="21"/>
+    <row r="107" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E107" s="18"/>
       <c r="F107" s="16"/>
       <c r="G107" s="16"/>
       <c r="H107" s="16"/>
       <c r="I107" s="16"/>
       <c r="J107" s="16"/>
       <c r="K107" s="17"/>
+      <c r="L107">
+        <f>SUM(F106:K107)</f>
+        <v>105</v>
+      </c>
     </row>
-    <row r="108" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E108" s="21" t="s">
+    <row r="108" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E108" s="18" t="s">
         <v>29</v>
       </c>
       <c r="F108" s="16">
         <v>10</v>
       </c>
       <c r="G108" s="16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H108" s="16">
         <v>0</v>
@@ -38137,62 +38028,48 @@
         <v>22</v>
       </c>
       <c r="K108" s="17">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="109" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E109" s="21"/>
+    <row r="109" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E109" s="18"/>
       <c r="F109" s="16"/>
       <c r="G109" s="16"/>
       <c r="H109" s="16"/>
       <c r="I109" s="16"/>
       <c r="J109" s="16"/>
       <c r="K109" s="17"/>
+      <c r="L109">
+        <f>SUM(F108:K109)</f>
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="J102:J103"/>
-    <mergeCell ref="K102:K103"/>
-    <mergeCell ref="J100:J101"/>
-    <mergeCell ref="K100:K101"/>
-    <mergeCell ref="J98:J99"/>
-    <mergeCell ref="K98:K99"/>
-    <mergeCell ref="J108:J109"/>
-    <mergeCell ref="K108:K109"/>
-    <mergeCell ref="J106:J107"/>
-    <mergeCell ref="K106:K107"/>
-    <mergeCell ref="J104:J105"/>
-    <mergeCell ref="K104:K105"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="G108:G109"/>
-    <mergeCell ref="H108:H109"/>
-    <mergeCell ref="I108:I109"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="G106:G107"/>
-    <mergeCell ref="H106:H107"/>
-    <mergeCell ref="I106:I107"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="G104:G105"/>
-    <mergeCell ref="H104:H105"/>
-    <mergeCell ref="I104:I105"/>
-    <mergeCell ref="E102:E103"/>
-    <mergeCell ref="F102:F103"/>
-    <mergeCell ref="G102:G103"/>
-    <mergeCell ref="H102:H103"/>
-    <mergeCell ref="I102:I103"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="F100:F101"/>
-    <mergeCell ref="G100:G101"/>
-    <mergeCell ref="H100:H101"/>
-    <mergeCell ref="I100:I101"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="F98:F99"/>
-    <mergeCell ref="G98:G99"/>
-    <mergeCell ref="H98:H99"/>
-    <mergeCell ref="I98:I99"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
     <mergeCell ref="J96:J97"/>
     <mergeCell ref="K96:K97"/>
     <mergeCell ref="H94:H95"/>
@@ -38207,30 +38084,48 @@
     <mergeCell ref="J94:J95"/>
     <mergeCell ref="K94:K95"/>
     <mergeCell ref="I96:I97"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="F98:F99"/>
+    <mergeCell ref="G98:G99"/>
+    <mergeCell ref="H98:H99"/>
+    <mergeCell ref="I98:I99"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="G100:G101"/>
+    <mergeCell ref="H100:H101"/>
+    <mergeCell ref="I100:I101"/>
+    <mergeCell ref="E102:E103"/>
+    <mergeCell ref="F102:F103"/>
+    <mergeCell ref="G102:G103"/>
+    <mergeCell ref="H102:H103"/>
+    <mergeCell ref="I102:I103"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="G104:G105"/>
+    <mergeCell ref="H104:H105"/>
+    <mergeCell ref="I104:I105"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="G106:G107"/>
+    <mergeCell ref="H106:H107"/>
+    <mergeCell ref="I106:I107"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="G108:G109"/>
+    <mergeCell ref="H108:H109"/>
+    <mergeCell ref="I108:I109"/>
+    <mergeCell ref="J108:J109"/>
+    <mergeCell ref="K108:K109"/>
+    <mergeCell ref="J106:J107"/>
+    <mergeCell ref="K106:K107"/>
+    <mergeCell ref="J104:J105"/>
+    <mergeCell ref="K104:K105"/>
+    <mergeCell ref="J102:J103"/>
+    <mergeCell ref="K102:K103"/>
+    <mergeCell ref="J100:J101"/>
+    <mergeCell ref="K100:K101"/>
+    <mergeCell ref="J98:J99"/>
+    <mergeCell ref="K98:K99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
[PdP] - Consuntivo aggiornato con differenza oraria (inizio vs fine).
</commit_message>
<xml_diff>
--- a/4 - RA/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
+++ b/4 - RA/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13800" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ARM" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="34">
   <si>
     <t>Francesco Bazzerla</t>
   </si>
@@ -873,11 +873,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2110379344"/>
-        <c:axId val="2110382848"/>
+        <c:axId val="2126578256"/>
+        <c:axId val="2126581792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110379344"/>
+        <c:axId val="2126578256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,7 +920,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110382848"/>
+        <c:crossAx val="2126581792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -928,7 +928,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110382848"/>
+        <c:axId val="2126581792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,7 +979,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110379344"/>
+        <c:crossAx val="2126578256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -993,7 +993,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2022,11 +2021,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2106305792"/>
-        <c:axId val="2106309328"/>
+        <c:axId val="2124694112"/>
+        <c:axId val="2124697664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2106305792"/>
+        <c:axId val="2124694112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2069,7 +2068,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106309328"/>
+        <c:crossAx val="2124697664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2077,7 +2076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106309328"/>
+        <c:axId val="2124697664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2128,7 +2127,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106305792"/>
+        <c:crossAx val="2124694112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2142,7 +2141,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3607,11 +3605,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2110646896"/>
-        <c:axId val="2110650432"/>
+        <c:axId val="2127114368"/>
+        <c:axId val="2127117904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110646896"/>
+        <c:axId val="2127114368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3654,7 +3652,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110650432"/>
+        <c:crossAx val="2127117904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3662,7 +3660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110650432"/>
+        <c:axId val="2127117904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3713,7 +3711,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110646896"/>
+        <c:crossAx val="2127114368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3727,7 +3725,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4048,9 +4045,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4069,9 +4064,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4090,9 +4083,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4162,9 +4153,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4257,7 +4246,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -4570,9 +4558,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4591,9 +4577,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4663,9 +4647,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4758,7 +4740,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -5363,11 +5344,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2109882896"/>
-        <c:axId val="2109879344"/>
+        <c:axId val="2095908656"/>
+        <c:axId val="2095912192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109882896"/>
+        <c:axId val="2095908656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5410,7 +5391,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109879344"/>
+        <c:crossAx val="2095912192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5418,7 +5399,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109879344"/>
+        <c:axId val="2095912192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5469,7 +5450,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109882896"/>
+        <c:crossAx val="2095908656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5483,7 +5464,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5783,9 +5763,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5855,9 +5833,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -5950,7 +5926,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6253,9 +6228,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6325,9 +6298,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6420,7 +6391,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -6757,9 +6727,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6842,7 +6810,6 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -7447,11 +7414,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2112025456"/>
-        <c:axId val="2112028992"/>
+        <c:axId val="2127244464"/>
+        <c:axId val="2127248000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2112025456"/>
+        <c:axId val="2127244464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7494,7 +7461,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112028992"/>
+        <c:crossAx val="2127248000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7502,7 +7469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112028992"/>
+        <c:axId val="2127248000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7553,7 +7520,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112025456"/>
+        <c:crossAx val="2127244464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7567,7 +7534,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10467,11 +10433,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="2112149408"/>
-        <c:axId val="2112152976"/>
+        <c:axId val="2127331872"/>
+        <c:axId val="2127335440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2112149408"/>
+        <c:axId val="2127331872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10514,7 +10480,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112152976"/>
+        <c:crossAx val="2127335440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10522,7 +10488,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112152976"/>
+        <c:axId val="2127335440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10573,7 +10539,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112149408"/>
+        <c:crossAx val="2127331872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10655,6 +10621,459 @@
 </file>
 
 <file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="20000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="265E91"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tot!$D$115:$D$126</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Project Manager </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Amministratore </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Analista </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Progettista </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Programmatore </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Verificatore </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tot!$E$115:$E$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-7.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:overlap val="100"/>
+        <c:axId val="2126426080"/>
+        <c:axId val="2126422480"/>
+      </c:barChart>
+      <c:valAx>
+        <c:axId val="2126422480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="95000"/>
+                      <a:lumOff val="5000"/>
+                      <a:alpha val="42000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="36000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2126426080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="2126426080"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2126422480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -10927,9 +11346,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -10948,9 +11365,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -10969,9 +11384,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -10990,9 +11403,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11011,9 +11422,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -11083,9 +11492,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -11188,7 +11595,6 @@
         <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -11258,7 +11664,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -11411,9 +11817,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -11452,7 +11856,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -11505,11 +11908,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2112230704"/>
-        <c:axId val="2112233632"/>
+        <c:axId val="2095984880"/>
+        <c:axId val="2095987808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2112230704"/>
+        <c:axId val="2095984880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11519,7 +11922,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112233632"/>
+        <c:crossAx val="2095987808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11527,7 +11930,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112233632"/>
+        <c:axId val="2095987808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11590,7 +11993,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112230704"/>
+        <c:crossAx val="2095984880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11638,7 +12041,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -12173,11 +12576,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="2112606976"/>
-        <c:axId val="-2144180848"/>
+        <c:axId val="2096059376"/>
+        <c:axId val="2096062960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2112606976"/>
+        <c:axId val="2096059376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12220,7 +12623,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144180848"/>
+        <c:crossAx val="2096062960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12228,7 +12631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144180848"/>
+        <c:axId val="2096062960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12279,7 +12682,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2112606976"/>
+        <c:crossAx val="2096059376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12293,7 +12696,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12658,9 +13060,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -12751,7 +13151,6 @@
         <c:idx val="9"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -13415,11 +13814,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2110483472"/>
-        <c:axId val="2110487008"/>
+        <c:axId val="2126737376"/>
+        <c:axId val="2126740912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110483472"/>
+        <c:axId val="2126737376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13462,7 +13861,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110487008"/>
+        <c:crossAx val="2126740912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13470,7 +13869,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110487008"/>
+        <c:axId val="2126740912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13521,7 +13920,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110483472"/>
+        <c:crossAx val="2126737376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13851,11 +14250,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="2111070544"/>
-        <c:axId val="2111074176"/>
+        <c:axId val="2126783056"/>
+        <c:axId val="2126786688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2111070544"/>
+        <c:axId val="2126783056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13893,7 +14292,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2111074176"/>
+        <c:crossAx val="2126786688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13901,7 +14300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111074176"/>
+        <c:axId val="2126786688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13964,7 +14363,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2111070544"/>
+        <c:crossAx val="2126783056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14542,11 +14941,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2110551328"/>
-        <c:axId val="2110554864"/>
+        <c:axId val="2126062784"/>
+        <c:axId val="2126066320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110551328"/>
+        <c:axId val="2126062784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14589,7 +14988,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110554864"/>
+        <c:crossAx val="2126066320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14597,7 +14996,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110554864"/>
+        <c:axId val="2126066320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14648,7 +15047,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110551328"/>
+        <c:crossAx val="2126062784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14662,7 +15061,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15683,11 +16081,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2111182752"/>
-        <c:axId val="2111186288"/>
+        <c:axId val="2126917856"/>
+        <c:axId val="2126921392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2111182752"/>
+        <c:axId val="2126917856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15730,7 +16128,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2111186288"/>
+        <c:crossAx val="2126921392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15738,7 +16136,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111186288"/>
+        <c:axId val="2126921392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15789,7 +16187,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2111182752"/>
+        <c:crossAx val="2126917856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15803,7 +16201,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17148,6 +17545,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors29.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -28272,7 +28709,7 @@
 </file>
 
 <file path=xl/charts/style27.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="218">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -28354,7 +28791,30 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -28364,15 +28824,29 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-          <a:alpha val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
@@ -28388,18 +28862,15 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -28413,18 +28884,15 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -28842,6 +29310,576 @@
 </file>
 
 <file path=xl/charts/style28.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="218">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style29.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -33419,6 +34457,84 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="Gruppo 14"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5676900" y="25107900"/>
+          <a:ext cx="8331200" cy="4622800"/>
+          <a:chOff x="5702300" y="25107900"/>
+          <a:chExt cx="8331200" cy="4622800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="4" name="Grafico 3"/>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="5702300" y="25107900"/>
+          <a:ext cx="8331200" cy="4622800"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="6" name="Connettore 1 5"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10515600" y="25361900"/>
+            <a:ext cx="0" cy="4203700"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -39209,10 +40325,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K109"/>
+  <dimension ref="A3:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D87" workbookViewId="0">
-      <selection activeCell="K92" sqref="K92"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E120" workbookViewId="0">
+      <selection activeCell="P123" sqref="P123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39801,8 +40917,86 @@
       <c r="J109" s="18"/>
       <c r="K109" s="19"/>
     </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D115" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E115" s="11">
+        <f>37-41</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D116" s="11"/>
+      <c r="E116" s="11"/>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D117" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E117" s="11">
+        <f>27-34</f>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D118" s="11"/>
+      <c r="E118" s="11"/>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D119" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E119" s="11">
+        <f>30-18</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D120" s="11"/>
+      <c r="E120" s="11"/>
+    </row>
+    <row r="121" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D121" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E121" s="11">
+        <f>232-248</f>
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D122" s="11"/>
+      <c r="E122" s="11"/>
+    </row>
+    <row r="123" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D123" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E123" s="11">
+        <f>150-132</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="124" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D124" s="11"/>
+      <c r="E124" s="11"/>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D125" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E125" s="11">
+        <f>259-255</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D126" s="11"/>
+      <c r="E126" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="80">
+  <mergeCells count="92">
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="A9:A10"/>
@@ -39883,6 +41077,18 @@
     <mergeCell ref="K100:K101"/>
     <mergeCell ref="J98:J99"/>
     <mergeCell ref="K98:K99"/>
+    <mergeCell ref="D115:D116"/>
+    <mergeCell ref="E115:E116"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="E117:E118"/>
+    <mergeCell ref="D119:D120"/>
+    <mergeCell ref="E119:E120"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="D123:D124"/>
+    <mergeCell ref="E123:E124"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="E125:E126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
[PdP] - Corretti errori nella trascrizione di alcuni valori nelle tabelle.
</commit_message>
<xml_diff>
--- a/4 - RA/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
+++ b/4 - RA/Esterni/Piano Di Progetto/GANTT-EXCEL/SWE-PianoDiLavoro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13800" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ARM" sheetId="1" r:id="rId1"/>
@@ -873,11 +873,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2126578256"/>
-        <c:axId val="2126581792"/>
+        <c:axId val="-2109608848"/>
+        <c:axId val="-2109526944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126578256"/>
+        <c:axId val="-2109608848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,7 +920,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126581792"/>
+        <c:crossAx val="-2109526944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -928,7 +928,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126581792"/>
+        <c:axId val="-2109526944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,7 +979,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126578256"/>
+        <c:crossAx val="-2109608848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -993,6 +993,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2021,11 +2022,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2124694112"/>
-        <c:axId val="2124697664"/>
+        <c:axId val="-2091046768"/>
+        <c:axId val="-2108914256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2124694112"/>
+        <c:axId val="-2091046768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2068,7 +2069,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124697664"/>
+        <c:crossAx val="-2108914256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2076,7 +2077,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124697664"/>
+        <c:axId val="-2108914256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2127,7 +2128,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124694112"/>
+        <c:crossAx val="-2091046768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2141,6 +2142,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3605,11 +3607,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2127114368"/>
-        <c:axId val="2127117904"/>
+        <c:axId val="2144540128"/>
+        <c:axId val="-2110889328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127114368"/>
+        <c:axId val="2144540128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3652,7 +3654,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127117904"/>
+        <c:crossAx val="-2110889328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3660,7 +3662,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127117904"/>
+        <c:axId val="-2110889328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3711,7 +3713,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127114368"/>
+        <c:crossAx val="2144540128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5344,11 +5346,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2095908656"/>
-        <c:axId val="2095912192"/>
+        <c:axId val="2142293248"/>
+        <c:axId val="2142337584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2095908656"/>
+        <c:axId val="2142293248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5391,7 +5393,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095912192"/>
+        <c:crossAx val="2142337584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5399,7 +5401,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2095912192"/>
+        <c:axId val="2142337584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5450,7 +5452,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095908656"/>
+        <c:crossAx val="2142293248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5464,6 +5466,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7414,11 +7417,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2127244464"/>
-        <c:axId val="2127248000"/>
+        <c:axId val="2140200784"/>
+        <c:axId val="-2110082016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127244464"/>
+        <c:axId val="2140200784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7461,7 +7464,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127248000"/>
+        <c:crossAx val="-2110082016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7469,7 +7472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127248000"/>
+        <c:axId val="-2110082016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7520,7 +7523,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127244464"/>
+        <c:crossAx val="2140200784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7534,6 +7537,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9008,7 +9012,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9027,7 +9033,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9046,7 +9054,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9065,7 +9075,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9084,7 +9096,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -9154,7 +9168,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -9257,6 +9273,7 @@
         <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -10433,11 +10450,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="2127331872"/>
-        <c:axId val="2127335440"/>
+        <c:axId val="-2108189888"/>
+        <c:axId val="-2109752256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127331872"/>
+        <c:axId val="-2108189888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10480,7 +10497,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127335440"/>
+        <c:crossAx val="-2109752256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10488,7 +10505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127335440"/>
+        <c:axId val="-2109752256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10539,7 +10556,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127331872"/>
+        <c:crossAx val="-2108189888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10918,11 +10935,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="2126426080"/>
-        <c:axId val="2126422480"/>
+        <c:axId val="2144036512"/>
+        <c:axId val="2141270736"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="2126422480"/>
+        <c:axId val="2141270736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10985,12 +11002,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126426080"/>
+        <c:crossAx val="2144036512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2126426080"/>
+        <c:axId val="2144036512"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -11009,7 +11026,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -11028,7 +11045,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126422480"/>
+        <c:crossAx val="2141270736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -11346,7 +11363,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11365,7 +11384,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11384,7 +11405,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11403,7 +11426,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11422,7 +11447,9 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -11492,7 +11519,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -11595,6 +11624,7 @@
         <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -11817,7 +11847,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -11856,6 +11888,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -11908,11 +11941,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2095984880"/>
-        <c:axId val="2095987808"/>
+        <c:axId val="-2119730832"/>
+        <c:axId val="2143926896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2095984880"/>
+        <c:axId val="-2119730832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11922,7 +11955,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095987808"/>
+        <c:crossAx val="2143926896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11930,7 +11963,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2095987808"/>
+        <c:axId val="2143926896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11993,7 +12026,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095984880"/>
+        <c:crossAx val="-2119730832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12576,11 +12609,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="2096059376"/>
-        <c:axId val="2096062960"/>
+        <c:axId val="-2110622400"/>
+        <c:axId val="-2110039376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2096059376"/>
+        <c:axId val="-2110622400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12623,7 +12656,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096062960"/>
+        <c:crossAx val="-2110039376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12631,7 +12664,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2096062960"/>
+        <c:axId val="-2110039376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12682,7 +12715,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096059376"/>
+        <c:crossAx val="-2110622400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12696,6 +12729,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13814,11 +13848,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2126737376"/>
-        <c:axId val="2126740912"/>
+        <c:axId val="2142345936"/>
+        <c:axId val="-2111231408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126737376"/>
+        <c:axId val="2142345936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13861,7 +13895,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126740912"/>
+        <c:crossAx val="-2111231408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13869,7 +13903,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126740912"/>
+        <c:axId val="-2111231408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13920,7 +13954,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126737376"/>
+        <c:crossAx val="2142345936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14175,6 +14209,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -14250,11 +14285,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="2126783056"/>
-        <c:axId val="2126786688"/>
+        <c:axId val="-2108704848"/>
+        <c:axId val="-2120042336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126783056"/>
+        <c:axId val="-2108704848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14292,7 +14327,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126786688"/>
+        <c:crossAx val="-2120042336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14300,7 +14335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126786688"/>
+        <c:axId val="-2120042336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14363,7 +14398,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126783056"/>
+        <c:crossAx val="-2108704848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14941,11 +14976,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2126062784"/>
-        <c:axId val="2126066320"/>
+        <c:axId val="2097073344"/>
+        <c:axId val="2096834640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126062784"/>
+        <c:axId val="2097073344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14988,7 +15023,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126066320"/>
+        <c:crossAx val="2096834640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14996,7 +15031,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126066320"/>
+        <c:axId val="2096834640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15047,7 +15082,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126062784"/>
+        <c:crossAx val="2097073344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15061,6 +15096,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16081,11 +16117,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2126917856"/>
-        <c:axId val="2126921392"/>
+        <c:axId val="2095103248"/>
+        <c:axId val="2095106560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126917856"/>
+        <c:axId val="2095103248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16128,7 +16164,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126921392"/>
+        <c:crossAx val="2095106560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16136,7 +16172,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126921392"/>
+        <c:axId val="2095106560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16187,7 +16223,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126917856"/>
+        <c:crossAx val="2095103248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16201,6 +16237,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -37362,10 +37399,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:J82"/>
+  <dimension ref="C4:J83"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="C64" zoomScaleNormal="187" zoomScalePageLayoutView="187" workbookViewId="0">
-      <selection activeCell="I88" sqref="I88"/>
+    <sheetView showRuler="0" topLeftCell="A62" zoomScaleNormal="187" zoomScalePageLayoutView="187" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37757,6 +37794,32 @@
       <c r="H82" s="18"/>
       <c r="I82" s="18"/>
       <c r="J82" s="19"/>
+    </row>
+    <row r="83" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="E83">
+        <f>SUM(E69:E82)</f>
+        <v>37</v>
+      </c>
+      <c r="F83">
+        <f>SUM(F69:F82)</f>
+        <v>27</v>
+      </c>
+      <c r="G83">
+        <f>SUM(G69:G82)</f>
+        <v>30</v>
+      </c>
+      <c r="H83">
+        <f>SUM(H69:H82)</f>
+        <v>232</v>
+      </c>
+      <c r="I83">
+        <f>SUM(I69:I82)</f>
+        <v>150</v>
+      </c>
+      <c r="J83">
+        <f>SUM(J69:J82)</f>
+        <v>259</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="78">
@@ -37906,7 +37969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="178" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" zoomScale="178" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -39446,7 +39509,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="138" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39860,7 +39923,7 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="113" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40325,10 +40388,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K126"/>
+  <dimension ref="A3:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="E120" workbookViewId="0">
-      <selection activeCell="P123" sqref="P123"/>
+    <sheetView showRuler="0" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="J112" sqref="J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40405,6 +40468,12 @@
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f>SUM(B3:B14)</f>
+        <v>734</v>
+      </c>
+    </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>15</v>
@@ -40476,6 +40545,12 @@
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="12"/>
       <c r="B54" s="11"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <f>SUM(B43:B54)</f>
+        <v>13621</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
@@ -40716,7 +40791,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E97" s="22"/>
       <c r="F97" s="18"/>
       <c r="G97" s="18"/>
@@ -40725,7 +40800,7 @@
       <c r="J97" s="18"/>
       <c r="K97" s="19"/>
     </row>
-    <row r="98" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E98" s="20" t="s">
         <v>24</v>
       </c>
@@ -40748,7 +40823,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E99" s="20"/>
       <c r="F99" s="18"/>
       <c r="G99" s="18"/>
@@ -40757,7 +40832,7 @@
       <c r="J99" s="18"/>
       <c r="K99" s="19"/>
     </row>
-    <row r="100" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E100" s="20" t="s">
         <v>25</v>
       </c>
@@ -40780,7 +40855,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E101" s="20"/>
       <c r="F101" s="18"/>
       <c r="G101" s="18"/>
@@ -40789,7 +40864,7 @@
       <c r="J101" s="18"/>
       <c r="K101" s="19"/>
     </row>
-    <row r="102" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E102" s="20" t="s">
         <v>26</v>
       </c>
@@ -40812,7 +40887,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E103" s="20"/>
       <c r="F103" s="18"/>
       <c r="G103" s="18"/>
@@ -40821,7 +40896,7 @@
       <c r="J103" s="18"/>
       <c r="K103" s="19"/>
     </row>
-    <row r="104" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E104" s="20" t="s">
         <v>27</v>
       </c>
@@ -40844,7 +40919,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="105" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E105" s="20"/>
       <c r="F105" s="18"/>
       <c r="G105" s="18"/>
@@ -40853,7 +40928,7 @@
       <c r="J105" s="18"/>
       <c r="K105" s="19"/>
     </row>
-    <row r="106" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E106" s="20" t="s">
         <v>28</v>
       </c>
@@ -40876,7 +40951,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="107" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E107" s="20"/>
       <c r="F107" s="18"/>
       <c r="G107" s="18"/>
@@ -40885,7 +40960,7 @@
       <c r="J107" s="18"/>
       <c r="K107" s="19"/>
     </row>
-    <row r="108" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E108" s="20" t="s">
         <v>29</v>
       </c>
@@ -40908,7 +40983,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E109" s="20"/>
       <c r="F109" s="18"/>
       <c r="G109" s="18"/>
@@ -40916,6 +40991,36 @@
       <c r="I109" s="18"/>
       <c r="J109" s="18"/>
       <c r="K109" s="19"/>
+    </row>
+    <row r="110" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F110">
+        <f>SUM(F96:F109)</f>
+        <v>37</v>
+      </c>
+      <c r="G110">
+        <f>SUM(G96:G109)</f>
+        <v>25</v>
+      </c>
+      <c r="H110">
+        <f>SUM(H96:H109)</f>
+        <v>30</v>
+      </c>
+      <c r="I110">
+        <f>SUM(I96:I109)</f>
+        <v>233</v>
+      </c>
+      <c r="J110">
+        <f>SUM(J96:J109)</f>
+        <v>152</v>
+      </c>
+      <c r="K110">
+        <f>SUM(K96:K109)</f>
+        <v>257</v>
+      </c>
+      <c r="L110">
+        <f>SUM(F110:K110)</f>
+        <v>734</v>
+      </c>
     </row>
     <row r="115" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D115" s="11" t="s">

</xml_diff>